<commit_message>
done push and sw
</commit_message>
<xml_diff>
--- a/instructions VS Csignals.xlsx
+++ b/instructions VS Csignals.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Collage\Arch\Project\Architecture_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVE\Desktop\first term 3\Architecture\ProjectArch\Architecture_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA966ACD-A61F-4745-BD47-97F8F0725AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADDD1EC3-347E-4994-B312-9F4D1C579A0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -230,7 +229,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -322,26 +321,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A7B7BB8-4A9C-487B-8331-2FB3AC2CED8B}" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0">
-  <autoFilter ref="A1:Q33" xr:uid="{6A7B7BB8-4A9C-487B-8331-2FB3AC2CED8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q33" totalsRowShown="0">
+  <autoFilter ref="A1:Q33"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7576037C-ACD3-43CB-B8A4-FDA1A2F5B622}" name="control signal"/>
-    <tableColumn id="2" xr3:uid="{116C7CAF-6E42-4DCF-B926-8347373D3DD1}" name="mem_read"/>
-    <tableColumn id="3" xr3:uid="{2C57975E-D1A4-4D5C-AFA0-440C7E4C3A7A}" name="immediate_value"/>
-    <tableColumn id="4" xr3:uid="{FAFDFC46-047A-4A45-8B7C-43F8284780BB}" name="branch"/>
-    <tableColumn id="5" xr3:uid="{26505D5F-EDA3-4794-8423-73F8CEBE0DC1}" name="mem_write"/>
-    <tableColumn id="6" xr3:uid="{04433103-C01F-4275-BF21-3A30F32E48DE}" name="reg_write1"/>
-    <tableColumn id="7" xr3:uid="{64D72DD0-4006-402F-BDE8-F9A1D8DCEB04}" name="reg_write2"/>
-    <tableColumn id="8" xr3:uid="{EFC9930E-9F21-402E-B9C7-4453D833DD2D}" name="reg_read1"/>
-    <tableColumn id="9" xr3:uid="{EE59E16E-55E3-499E-B684-2E8EA97D6D4D}" name="reg_read2"/>
-    <tableColumn id="10" xr3:uid="{EA853F61-1A6C-48C6-806B-A8396C0BD9BD}" name="reg_read3"/>
-    <tableColumn id="11" xr3:uid="{848BCE0B-41C9-4D83-8026-4A209D633C0C}" name="stack_read"/>
-    <tableColumn id="12" xr3:uid="{C66A4BA4-7C8C-4B7F-AD34-345E329757DE}" name="stack_write"/>
-    <tableColumn id="21" xr3:uid="{61A6AAC1-6BE6-4F1D-9F3B-8B3C2C541246}" name="protectAfree"/>
-    <tableColumn id="22" xr3:uid="{A9A25248-86F8-4F20-BDB2-6A3E7E79A3B7}" name="protectOfree"/>
-    <tableColumn id="25" xr3:uid="{6C59EB52-99DB-4A0F-A34B-0FD07C49268D}" name="inOout"/>
-    <tableColumn id="24" xr3:uid="{B9EBD68E-15EE-4B78-A006-A10F2AB722F5}" name="inAout"/>
-    <tableColumn id="13" xr3:uid="{0640AE2B-03E1-4D5F-BC25-3F6EB4274EC2}" name="alu_op" dataDxfId="0"/>
+    <tableColumn id="1" name="control signal"/>
+    <tableColumn id="2" name="mem_read"/>
+    <tableColumn id="3" name="immediate_value"/>
+    <tableColumn id="4" name="branch"/>
+    <tableColumn id="5" name="mem_write"/>
+    <tableColumn id="6" name="reg_write1"/>
+    <tableColumn id="7" name="reg_write2"/>
+    <tableColumn id="8" name="reg_read1"/>
+    <tableColumn id="9" name="reg_read2"/>
+    <tableColumn id="10" name="reg_read3"/>
+    <tableColumn id="11" name="stack_read"/>
+    <tableColumn id="12" name="stack_write"/>
+    <tableColumn id="21" name="protectAfree"/>
+    <tableColumn id="22" name="protectOfree"/>
+    <tableColumn id="25" name="inOout"/>
+    <tableColumn id="24" name="inAout"/>
+    <tableColumn id="13" name="alu_op" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -643,11 +642,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BFE430-AD0B-438B-AC73-F73F102B6F5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:M8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>

</xml_diff>